<commit_message>
Add geração de xlsx com erro
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -206,8 +206,8 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="#"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -234,21 +234,59 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,6 +316,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -285,92 +361,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -386,31 +386,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,25 +500,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,7 +530,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,7 +542,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,97 +560,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,6 +577,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -600,30 +624,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -682,142 +682,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1158,7 +1158,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -1306,7 +1306,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="3">
-        <v>43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1460,7 +1460,7 @@
         <v>54</v>
       </c>
       <c r="C27" s="3">
-        <v>57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3">

</xml_diff>